<commit_message>
Added swagger response attributes. Corrected email arguments to be query parameters rather than path parameters due to 404 status code issue.
</commit_message>
<xml_diff>
--- a/Test-Results.xlsx
+++ b/Test-Results.xlsx
@@ -9,11 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
-    <sheet name="Attachment" sheetId="2" r:id="rId2"/>
+    <sheet name="Contact" sheetId="3" r:id="rId2"/>
+    <sheet name="Contract" sheetId="4" r:id="rId3"/>
+    <sheet name="Attachment" sheetId="2" r:id="rId4"/>
+    <sheet name="Resource" sheetId="7" r:id="rId5"/>
+    <sheet name="Note" sheetId="5" r:id="rId6"/>
+    <sheet name="Picklist" sheetId="6" r:id="rId7"/>
+    <sheet name="Generic" sheetId="8" r:id="rId8"/>
+    <sheet name="Task" sheetId="9" r:id="rId9"/>
+    <sheet name="Ticket" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
   <si>
     <t>Operation</t>
   </si>
@@ -34,9 +42,6 @@
   </si>
   <si>
     <t>Request URL</t>
-  </si>
-  <si>
-    <t>http://localhost:56786/api/account/GetByName/standard</t>
   </si>
   <si>
     <t>OK</t>
@@ -49,43 +54,279 @@
 </t>
   </si>
   <si>
-    <t>http://localhost:56786/api/account/GetByLastActivityDate/2017-02-03</t>
-  </si>
-  <si>
     <t>GET /api/account/GetByNumber/{accountNumber}</t>
   </si>
   <si>
-    <t>http://localhost:56786/api/account/GetByNumber/0</t>
-  </si>
-  <si>
     <t>GET /api/account/GetById/{id}</t>
   </si>
   <si>
-    <t>http://localhost:56786/api/account/GetById/174</t>
-  </si>
-  <si>
     <t>GET /api/attachment/GetInfoByParentId/{parentId}</t>
   </si>
   <si>
-    <t>http://localhost:56786/api/attachment/GetInfoByParentId/14146</t>
-  </si>
-  <si>
     <t>GET /api/attachment/GetById/{id}</t>
   </si>
   <si>
-    <t>http://localhost:56786/api/attachment/GetById/363</t>
-  </si>
-  <si>
     <t>GET /api/attachment/GetInfoByAttachDate/{attachDate}</t>
   </si>
   <si>
-    <t>http://localhost:56786/api/attachment/GetInfoByAttachDate/2016-12-27</t>
-  </si>
-  <si>
     <t>GET /api/attachment/GetInfoByParentIdAndAttachDate/{parentId}/{attachDate}</t>
   </si>
   <si>
-    <t>http://localhost:56786/api/attachment/GetInfoByParentIdAndAttachDate/14141/2017-02-01</t>
+    <t>GET /api/contact/GetById/{id}</t>
+  </si>
+  <si>
+    <t>GET /api/contact/GetByName/{firstName}/{lastName}</t>
+  </si>
+  <si>
+    <t>GET /api/contact/GetByEmail</t>
+  </si>
+  <si>
+    <t>GET /api/contact/GetByAccountId/{accountId}</t>
+  </si>
+  <si>
+    <t>GET /api/contract/GetById/{id}</t>
+  </si>
+  <si>
+    <t>GET /api/contract/GetByContactId/{contactId}</t>
+  </si>
+  <si>
+    <t>GET /api/contract/GetByAccountId/{accountId}</t>
+  </si>
+  <si>
+    <t>GET /api/contract/GetByOpportunityId/{opportunityId}</t>
+  </si>
+  <si>
+    <t>GET /api/note/GetByTicketId/{ticketId}</t>
+  </si>
+  <si>
+    <t>GET /api/note/GetById/{id}</t>
+  </si>
+  <si>
+    <t>GET /api/note/GetByLastActivityDate/{lastActivityDate}</t>
+  </si>
+  <si>
+    <t>{
+  "ticketId": 14177,
+  "creatorResourceId": 29683366,
+  "title": "test note",
+  "description": "test note",
+  "noteType": 3,
+  "publish": 1
+}</t>
+  </si>
+  <si>
+    <t>POST /api/note/PostTicketNote</t>
+  </si>
+  <si>
+    <t>OK 29729317</t>
+  </si>
+  <si>
+    <t>GET /api/picklist/GetLabel/{entityType}/{fieldName}/{valueToSearch}</t>
+  </si>
+  <si>
+    <t>"In Progress"</t>
+  </si>
+  <si>
+    <t>GET /api/picklist/GetLabels/{entityType}/{fieldName}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetById/{id}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetByName/{firstName}/{lastName}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetByEmail</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetByUsername/{userName}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetByLocationId/{locationId}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetRoleByResourceId/{resourceId}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetRoleById/{roleId}</t>
+  </si>
+  <si>
+    <t>GET /api/resource/GetAllRoles</t>
+  </si>
+  <si>
+    <t>Post Body, if applicable</t>
+  </si>
+  <si>
+    <t>Post Body if applicable</t>
+  </si>
+  <si>
+    <t>GET /api/generic/GetByEntityNameFieldNameAndValue</t>
+  </si>
+  <si>
+    <t>GET /api/task/GetByProjectId/{projectId}</t>
+  </si>
+  <si>
+    <t>GET /api/task/GetById/{id}</t>
+  </si>
+  <si>
+    <t>GET /api/task/GetByCreatorResourceId/{creatorResourceId}</t>
+  </si>
+  <si>
+    <t>GET /api/task/GetByLastActivityDate/{lastActivityDate}</t>
+  </si>
+  <si>
+    <t>GET /api/task/GetByProjectIdAndStatus/{projectId}/{status}</t>
+  </si>
+  <si>
+    <t>GET /api/task/GetByProjectIdAndPriority/{projectId}/{priority}</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/account/GetByName/standard</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/account/GetByLastActivityDate/2017-02-03</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/account/GetByNumber/0</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/account/GetById/174</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contact/GetById/31716564</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contact/GetByName/Mukumadi/Tshibuabua</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contact/GetByEmail/pmponzi%40tceglobal.com</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contact/GetByAccountId/29683317</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contract/GetById/29685870</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contract/GetByContactId/29683319</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contract/GetByAccountId/0</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/contract/GetByOpportunityId/29712482</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/attachment/GetInfoByParentId/14146</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/attachment/GetById/363</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/attachment/GetInfoByAttachDate/2016-12-27</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/attachment/GetInfoByParentIdAndAttachDate/14141/2017-02-01</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetById/29682885</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetByName/Paul/Mponzi</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetByEmail?email=pmponzi%40tceglobal.net</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetByUsername/pmponzi</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetByLocationId/90682</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetRoleByResourceId/29682885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Your API Base URL}/api/resource/GetRoleById/29686374
+</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/resource/GetAllRoles</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/note/GetByTicketId/14146</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/note/GetById/29729225</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/note/GetByLastActivityDate/2017-02-01</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/note/PostTicketNote</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/picklist/GetLabel/Ticket/Status/8</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/picklist/GetLabels/Ticket/Status</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/generic/GetByEntityNameFieldNameAndValue?entityName=Ticket&amp;fieldName=id&amp;fieldValue=14177</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/task/GetByProjectId/19</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/task/GetById/14195</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/task/GetByCreatorResourceId/30716561</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/task/GetByLastActivityDate/2017-01-31</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/task/GetByProjectIdAndStatus/17/5</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/task/GetByProjectIdAndPriority/17/0</t>
+  </si>
+  <si>
+    <t>GET /api/ticket/GetByAccountId/{accountId}</t>
+  </si>
+  <si>
+    <t>GET /api/ticket/GetById/{id}</t>
+  </si>
+  <si>
+    <t>GET /api/ticket/GetByCreatorResourceId/{creatorResourceId}</t>
+  </si>
+  <si>
+    <t>GET /api/ticket/GetByLastActivityDate/{lastActivityDate}</t>
+  </si>
+  <si>
+    <t>GET /api/ticket/GetByAccountIdAndStatus/{accountId}/{status}</t>
+  </si>
+  <si>
+    <t>GET /api/ticket/GetByAccountIdAndPriority/{accountId}/{priority}</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/ticket/GetByAccountId/29685975</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/ticket/GetById/7966</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/ticket/GetByCreatorResourceId/29682885</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/ticket/GetByLastActivityDate/2017-02-01</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/ticket/GetByAccountIdAndStatus/29685975/5</t>
+  </si>
+  <si>
+    <t>{Your API Base URL}/api/ticket/GetByAccountIdAndPriority/29685975/6</t>
   </si>
 </sst>
 </file>
@@ -109,12 +350,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FF880000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,11 +373,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -147,12 +385,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,19 +720,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -487,68 +743,331 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
+      <c r="B5" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://localhost:56786/api/account/GetByLastActivityDate/2017-02-03"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://localhost:56786/api/account/GetByNumber/0"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,9 +1075,10 @@
     <col min="1" max="1" width="28.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -568,58 +1088,464 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" style="7" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>